<commit_message>
add photo to new and list of defect
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CDU_coding\HIT137-SoftwareNow_Code\road-defect-management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B4D76FA-7D4C-42CA-9B85-E30066AF170C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F779205-30FF-4198-A421-F9BC0AAC8AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B3D3EF61-2CD7-41AD-AE32-96472ED5B6AE}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="55">
   <si>
     <t>Trower road</t>
   </si>
@@ -182,9 +182,6 @@
     <t>ada</t>
   </si>
   <si>
-    <t xml:space="preserve">Road new </t>
-  </si>
-  <si>
     <t>Road11 allala</t>
   </si>
   <si>
@@ -192,6 +189,22 @@
   </si>
   <si>
     <t>asdasdsa</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>hi there_x000D_
+hi bro</t>
+  </si>
+  <si>
+    <t>Road new</t>
+  </si>
+  <si>
+    <t>OOOAO</t>
+  </si>
+  <si>
+    <t>ooasodo</t>
   </si>
 </sst>
 </file>
@@ -233,9 +246,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652EA00B-8DFE-4FD8-B8C8-ADCE90BC0D58}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +593,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -615,7 +631,12 @@
       <c r="G2" s="1">
         <v>44206</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1">
+        <v>44863</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
       <c r="J2">
         <v>0</v>
       </c>
@@ -637,12 +658,15 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1">
         <v>44207</v>
       </c>
       <c r="H3" s="1"/>
+      <c r="I3" t="s">
+        <v>50</v>
+      </c>
       <c r="J3">
         <v>0</v>
       </c>
@@ -728,6 +752,9 @@
       <c r="H6" s="1">
         <v>44212</v>
       </c>
+      <c r="I6" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="J6">
         <v>0</v>
       </c>
@@ -1174,11 +1201,11 @@
       <c r="D22" t="s">
         <v>2</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>25</v>
       </c>
       <c r="G22" t="s">
         <v>34</v>
@@ -1331,10 +1358,10 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" t="s">
         <v>47</v>
-      </c>
-      <c r="C28" t="s">
-        <v>48</v>
       </c>
       <c r="D28" t="s">
         <v>2</v>
@@ -1360,7 +1387,7 @@
         <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
         <v>24</v>
@@ -1378,9 +1405,41 @@
         <v>44862</v>
       </c>
       <c r="I29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="1">
+        <v>44863</v>
+      </c>
+      <c r="H30" s="1">
+        <v>44863</v>
+      </c>
+      <c r="I30">
+        <v>22222</v>
+      </c>
+      <c r="J30">
         <v>0</v>
       </c>
     </row>

</xml_diff>